<commit_message>
finished Python and SQL
</commit_message>
<xml_diff>
--- a/results/answers.xlsx
+++ b/results/answers.xlsx
@@ -14,12 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>Số đã bán</t>
   </si>
   <si>
-    <t>Tổng doanh số</t>
+    <t>Doanh số</t>
   </si>
   <si>
     <t>Thương hiệu</t>
@@ -98,18 +98,6 @@
   </si>
   <si>
     <t>samsung galaxy s23</t>
-  </si>
-  <si>
-    <t>Doanh số theo hãng</t>
-  </si>
-  <si>
-    <t>Điện thoại Trung Quốc bán chạy nhất</t>
-  </si>
-  <si>
-    <t>Doanh số bán điện thoại của Mỹ là tốt nhất</t>
-  </si>
-  <si>
-    <t>Tỉ lệ doanh số và số đã bán của S23 so với các mẫu khác của Samsung</t>
   </si>
 </sst>
 </file>
@@ -467,313 +455,302 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" t="s">
-        <v>31</v>
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>6802</v>
+      </c>
+      <c r="C2">
+        <v>180426979000</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2">
+        <v>24484</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2">
+        <v>181464022000</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>47.61</v>
+      </c>
+      <c r="M2">
+        <v>52.39</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>17</v>
+      </c>
+      <c r="C3">
+        <v>445230000</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3">
+        <v>23824</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3">
+        <v>162307444133</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>27</v>
+      <c r="L3">
+        <v>82.23</v>
+      </c>
+      <c r="M3">
+        <v>17.77</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>6802</v>
+        <v>392</v>
       </c>
       <c r="C4">
-        <v>765358458000</v>
+        <v>1037043000</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4">
+        <v>7194</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F4">
-        <v>24292</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="I4">
-        <v>777585049000</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>0.61</v>
-      </c>
-      <c r="M4">
-        <v>0.39</v>
+        <v>140975520017</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>17</v>
+        <v>288</v>
       </c>
       <c r="C5">
-        <v>628560000</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5">
-        <v>23824</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5">
-        <v>744591130261</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0.82</v>
-      </c>
-      <c r="M5">
-        <v>0.18</v>
+        <v>797035000</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>392</v>
+        <v>152</v>
       </c>
       <c r="C6">
-        <v>12226591000</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6">
-        <v>7194</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6">
-        <v>443902753370</v>
+        <v>384880000</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7">
-        <v>288</v>
+        <v>161</v>
       </c>
       <c r="C7">
-        <v>2217190000</v>
+        <v>207986240</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>152</v>
+        <v>1433</v>
       </c>
       <c r="C8">
-        <v>1013554000</v>
+        <v>1953184000</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B9">
-        <v>161</v>
+        <v>577</v>
       </c>
       <c r="C9">
-        <v>602261760</v>
+        <v>290433000</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>1433</v>
+        <v>7667</v>
       </c>
       <c r="C10">
-        <v>74030165620</v>
+        <v>10192371140</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>577</v>
+        <v>18</v>
       </c>
       <c r="C11">
-        <v>869951000</v>
+        <v>233820000</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B12">
-        <v>7667</v>
+        <v>1619</v>
       </c>
       <c r="C12">
-        <v>80207736369</v>
+        <v>4359920556</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13">
-        <v>18</v>
+        <v>192</v>
       </c>
       <c r="C13">
-        <v>689880000</v>
+        <v>1291847000</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B14">
-        <v>1619</v>
+        <v>22391</v>
       </c>
       <c r="C14">
-        <v>14182803910</v>
+        <v>160354260133</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B15">
-        <v>192</v>
+        <v>1763</v>
       </c>
       <c r="C15">
-        <v>2854049996</v>
+        <v>2494325860</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B16">
-        <v>22391</v>
+        <v>36</v>
       </c>
       <c r="C16">
-        <v>670560964641</v>
+        <v>179640000</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B17">
-        <v>1763</v>
+        <v>1452</v>
       </c>
       <c r="C17">
-        <v>47427404270</v>
+        <v>1102149000</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B18">
-        <v>36</v>
+        <v>1764</v>
       </c>
       <c r="C18">
-        <v>971070000</v>
+        <v>1143591000</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B19">
-        <v>1452</v>
+        <v>464</v>
       </c>
       <c r="C19">
-        <v>1102149000</v>
+        <v>255598000</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B20">
-        <v>1764</v>
+        <v>12587</v>
       </c>
       <c r="C20">
-        <v>6203344000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <v>464</v>
-      </c>
-      <c r="C21">
-        <v>818154800</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22">
-        <v>12587</v>
-      </c>
-      <c r="C22">
-        <v>337814913331</v>
+        <v>122184429081</v>
       </c>
     </row>
   </sheetData>

</xml_diff>